<commit_message>
Add link to presentation, rerun notebooks, add some fields to INDEC and INE excels list.
</commit_message>
<xml_diff>
--- a/3-excel_links/ARG_INDEC.xlsx
+++ b/3-excel_links/ARG_INDEC.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr/>
-  <s:bookViews>
-    <s:workbookView activeTab="0"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="download_links" sheetId="1" r:id="rId1"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+  <workbookPr autoCompressPictures="0"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="1080" windowWidth="25600" windowHeight="14980"/>
+  </bookViews>
+  <sheets>
+    <sheet name="download_links" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1059">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2347" uniqueCount="1066">
   <si>
     <t>description</t>
   </si>
@@ -3191,25 +3196,52 @@
   </si>
   <si>
     <t>codigos_prov_depto_censo2010.xls</t>
+  </si>
+  <si>
+    <t>categories</t>
+  </si>
+  <si>
+    <t>headers_coord</t>
+  </si>
+  <si>
+    <t>data_starts</t>
+  </si>
+  <si>
+    <t>frequency</t>
+  </si>
+  <si>
+    <t>time_header_coord</t>
+  </si>
+  <si>
+    <t>context</t>
+  </si>
+  <si>
+    <t>ws_name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -3225,16 +3257,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -3522,31 +3555,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:sheetPr>
-    <s:outlinePr summaryBelow="1" summaryRight="1"/>
-    <s:pageSetUpPr/>
-  </s:sheetPr>
-  <dimension ref="A1:C780"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J780"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>1059</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1060</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1061</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1062</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1063</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3557,7 +3607,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3568,7 +3618,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3579,7 +3629,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -3590,7 +3640,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -3601,7 +3651,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -3612,7 +3662,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -3623,7 +3673,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -3634,7 +3684,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -3645,7 +3695,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -3656,7 +3706,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -3667,7 +3717,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -3678,7 +3728,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -3689,7 +3739,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -3700,7 +3750,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -12116,6 +12166,11 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>